<commit_message>
[Distiller] Update water flow calculator.
</commit_message>
<xml_diff>
--- a/distiller/domain/doc/water_flow_sensor.xlsx
+++ b/distiller/domain/doc/water_flow_sensor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prj\dev-test\sources\arduino\arduino-projects\arduino-sandbox\distiller\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prj\dev-test\sources\java\java-sandbox\distiller\domain\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Sensor's RPM</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Calculated flow[l/h]</t>
+  </si>
+  <si>
+    <t>Old calculated flow [l/h]</t>
   </si>
 </sst>
 </file>
@@ -256,102 +259,54 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$15</c:f>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>380</c:v>
+                  <c:v>458</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>420</c:v>
+                  <c:v>1025</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1080</c:v>
+                  <c:v>1450</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1260</c:v>
+                  <c:v>2141</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1320</c:v>
+                  <c:v>2863</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1860</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2340</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2400</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3180</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3240</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4380</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4440</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4500</c:v>
+                  <c:v>3760</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$15</c:f>
+              <c:f>Sheet1!$E$2:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5.0279329608938541</c:v>
+                  <c:v>13.714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0279329608938541</c:v>
+                  <c:v>13.584905660377359</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.594594594594595</c:v>
+                  <c:v>17.777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.744186046511629</c:v>
+                  <c:v>25.263157894736842</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.744186046511629</c:v>
+                  <c:v>31.304347826086957</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.225806451612904</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>23.225806451612904</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>29.189189189189189</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>29.189189189189189</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>38.571428571428577</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>38.571428571428577</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>52.173913043478258</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>52.173913043478258</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>52.173913043478258</c:v>
+                  <c:v>42.352941176470594</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1135,15 +1090,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>659130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1429,10 +1384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1442,9 +1397,10 @@
     <col min="3" max="3" width="10.109375" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1461,271 +1417,146 @@
         <v>4</v>
       </c>
       <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>380</v>
+        <v>458</v>
       </c>
       <c r="B2">
-        <v>125</v>
+        <v>200</v>
       </c>
       <c r="C2">
-        <v>89.5</v>
+        <v>52.5</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D15" si="0">60*$B2/1000/$C2</f>
-        <v>8.3798882681564241E-2</v>
+        <f t="shared" ref="D2:D7" si="0">60*$B2/1000/$C2</f>
+        <v>0.22857142857142856</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E15" si="1">60*$D2</f>
-        <v>5.0279329608938541</v>
+        <f t="shared" ref="E2:E7" si="1">60*$D2</f>
+        <v>13.714285714285714</v>
+      </c>
+      <c r="G2">
+        <f>0.0115 * $A2 + 1.6001</f>
+        <v>6.8671000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>420</v>
+        <v>1025</v>
       </c>
       <c r="B3">
-        <v>125</v>
+        <v>200</v>
       </c>
       <c r="C3">
-        <v>89.5</v>
+        <v>53</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>8.3798882681564241E-2</v>
+        <v>0.22641509433962265</v>
       </c>
       <c r="E3">
         <f t="shared" si="1"/>
-        <v>5.0279329608938541</v>
+        <v>13.584905660377359</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="2">0.0115 * $A3 + 1.6001</f>
+        <v>13.387599999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1080</v>
+        <v>1450</v>
       </c>
       <c r="B4">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C4">
-        <v>74</v>
+        <v>40.5</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>0.24324324324324326</v>
+        <v>0.29629629629629628</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>14.594594594594595</v>
+        <v>17.777777777777779</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>18.275100000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1260</v>
+        <v>2141</v>
       </c>
       <c r="B5">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C5">
-        <v>64.5</v>
+        <v>28.5</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0.27906976744186046</v>
+        <v>0.42105263157894735</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>16.744186046511629</v>
+        <v>25.263157894736842</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>26.221600000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1320</v>
+        <v>2863</v>
       </c>
       <c r="B6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C6">
-        <v>64.5</v>
+        <v>23</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0.27906976744186046</v>
+        <v>0.52173913043478259</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>16.744186046511629</v>
+        <v>31.304347826086957</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>34.5246</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1800</v>
+        <v>3760</v>
       </c>
       <c r="B7">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C7">
-        <v>46.5</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.38709677419354838</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>23.225806451612904</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1860</v>
-      </c>
-      <c r="B8">
-        <v>300</v>
-      </c>
-      <c r="C8">
-        <v>46.5</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0.38709677419354838</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>23.225806451612904</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2340</v>
-      </c>
-      <c r="B9">
-        <v>300</v>
-      </c>
-      <c r="C9">
-        <v>37</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0.48648648648648651</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>29.189189189189189</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2400</v>
-      </c>
-      <c r="B10">
-        <v>300</v>
-      </c>
-      <c r="C10">
-        <v>37</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0.48648648648648651</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>29.189189189189189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>3180</v>
-      </c>
-      <c r="B11">
-        <v>300</v>
-      </c>
-      <c r="C11">
-        <v>28</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>0.6428571428571429</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>38.571428571428577</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>3240</v>
-      </c>
-      <c r="B12">
-        <v>300</v>
-      </c>
-      <c r="C12">
-        <v>28</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0.6428571428571429</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>38.571428571428577</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>4380</v>
-      </c>
-      <c r="B13">
-        <v>300</v>
-      </c>
-      <c r="C13">
-        <v>20.7</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0.86956521739130432</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>52.173913043478258</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>4440</v>
-      </c>
-      <c r="B14">
-        <v>300</v>
-      </c>
-      <c r="C14">
-        <v>20.7</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0.86956521739130432</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>52.173913043478258</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>4500</v>
-      </c>
-      <c r="B15">
-        <v>300</v>
-      </c>
-      <c r="C15">
-        <v>20.7</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0.86956521739130432</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>52.173913043478258</v>
+        <v>42.352941176470594</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>44.8401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>